<commit_message>
more organization and planning work done
</commit_message>
<xml_diff>
--- a/gp-services/ReportOutPlanning.xlsx
+++ b/gp-services/ReportOutPlanning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dconly\GitRepos\PPA3\gp-services\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73F4CB69-6790-46BD-BA30-9CCA8B428886}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28460CA9-96AD-4DB9-9A2B-C60679167979}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
     <sheet name="check" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">ChartRoster!$A$1:$F$31</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">ChartRoster!$A$1:$F$71</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="206">
   <si>
     <t>Program</t>
   </si>
@@ -202,15 +202,6 @@
     <t>JSON Generator script and JSON template</t>
   </si>
   <si>
-    <t>RP_ARTEXP_VMT</t>
-  </si>
-  <si>
-    <t>RP_ARTEXP_SGR</t>
-  </si>
-  <si>
-    <t>RP_ARTEXP_CONG</t>
-  </si>
-  <si>
     <t>NOTE - THIS IS FOR REPLICATING CURRENT TOOL; NOT IMPLEMENTING ANY WISH LIST CHANGES</t>
   </si>
   <si>
@@ -241,9 +232,6 @@
     <t>ArterialSGR</t>
   </si>
   <si>
-    <t>RP_ARTSGR_CONG</t>
-  </si>
-  <si>
     <t xml:space="preserve">Example: </t>
   </si>
   <si>
@@ -283,21 +271,12 @@
     <t>Map</t>
   </si>
   <si>
-    <t>RP_ARTEXP_MM</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
     <t>Same as RP_ARTEXP_CONG except doesn't have job + du chart</t>
   </si>
   <si>
-    <t>RP_ARTEXP_ECON</t>
-  </si>
-  <si>
-    <t>RP_ARTSGR_ECON</t>
-  </si>
-  <si>
     <t>Same as RP_ARTEXP_ECON, but doesn't have "new jobs added" number</t>
   </si>
   <si>
@@ -319,12 +298,6 @@
     <t>ChartName must be unique to each chart.</t>
   </si>
   <si>
-    <t>RP_ARTEXP_FRGT</t>
-  </si>
-  <si>
-    <t>RP_ARTSGR_FRGT</t>
-  </si>
-  <si>
     <t>Same as RP_ARTEXP_FRGT but doesn't have chart showing change in industrial jobs</t>
   </si>
   <si>
@@ -343,9 +316,6 @@
     <t>ChangeIndJobs</t>
   </si>
   <si>
-    <t>RP_ARTEXP_SAF</t>
-  </si>
-  <si>
     <t>TotCollision</t>
   </si>
   <si>
@@ -364,9 +334,6 @@
     <t>ATFCollShare</t>
   </si>
   <si>
-    <t>RP_ARTSGR_SGR</t>
-  </si>
-  <si>
     <t>PCI</t>
   </si>
   <si>
@@ -379,24 +346,6 @@
     <t>PctEJPop</t>
   </si>
   <si>
-    <t>RP_FWY_CONG</t>
-  </si>
-  <si>
-    <t>RP_FWY_VMT</t>
-  </si>
-  <si>
-    <t>RP_FWY_MM</t>
-  </si>
-  <si>
-    <t>RP_FWY_ECON</t>
-  </si>
-  <si>
-    <t>RP_FWY_FRGT</t>
-  </si>
-  <si>
-    <t>RP_FWY_SAF</t>
-  </si>
-  <si>
     <t>TransitTrips</t>
   </si>
   <si>
@@ -538,39 +487,21 @@
     <t>TransportationChoice</t>
   </si>
   <si>
-    <t>CD_TRNCHOICE</t>
-  </si>
-  <si>
     <t>CompactDev</t>
   </si>
   <si>
-    <t>CD_COMPACTDEV</t>
-  </si>
-  <si>
     <t>MixedUse</t>
   </si>
   <si>
-    <t>CD_MIXEDUSE</t>
-  </si>
-  <si>
     <t>HousingChoice</t>
   </si>
   <si>
-    <t>CD_HOUSCHOICE</t>
-  </si>
-  <si>
     <t>ExistingAssets</t>
   </si>
   <si>
-    <t>CD_EXISTGASSET</t>
-  </si>
-  <si>
     <t>NaturePreservation</t>
   </si>
   <si>
-    <t>CD_NATURPRES</t>
-  </si>
-  <si>
     <t>tbd as of 2/24/2022</t>
   </si>
   <si>
@@ -661,9 +592,6 @@
     <t>shared-modules</t>
   </si>
   <si>
-    <t>Modules and functions that can be copy/pasted across sub reports</t>
-  </si>
-  <si>
     <t>rp_title</t>
   </si>
   <si>
@@ -740,6 +668,15 @@
   </si>
   <si>
     <t>cd_naturpres</t>
+  </si>
+  <si>
+    <t>&lt;other Modules and functions that can be copy/pasted across sub reports&gt;</t>
+  </si>
+  <si>
+    <t>chartbuilders</t>
+  </si>
+  <si>
+    <t>functions and classes for updating JSON portions for charts used in multiple reports</t>
   </si>
 </sst>
 </file>
@@ -2188,7 +2125,7 @@
   <dimension ref="A1:X44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2203,7 +2140,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
@@ -2365,122 +2302,128 @@
     <row r="25" spans="1:24" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>186</v>
+        <v>163</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>190</v>
+        <v>167</v>
       </c>
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>178</v>
+        <v>155</v>
       </c>
       <c r="O28" t="s">
-        <v>183</v>
+        <v>160</v>
       </c>
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>185</v>
+        <v>162</v>
       </c>
       <c r="P29" t="s">
-        <v>193</v>
+        <v>170</v>
       </c>
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
-        <v>199</v>
+        <v>176</v>
       </c>
       <c r="Q30" t="s">
-        <v>195</v>
+        <v>172</v>
       </c>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="P31" t="s">
-        <v>194</v>
+        <v>171</v>
       </c>
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="C32" t="s">
-        <v>183</v>
-      </c>
       <c r="E32" t="s">
-        <v>189</v>
+        <v>205</v>
       </c>
       <c r="Q32" t="s">
-        <v>196</v>
+        <v>173</v>
       </c>
     </row>
     <row r="33" spans="2:17" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="O33" t="s">
-        <v>184</v>
+        <v>161</v>
       </c>
     </row>
     <row r="34" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>160</v>
+      </c>
+      <c r="E34" t="s">
+        <v>166</v>
+      </c>
       <c r="P34" t="s">
-        <v>193</v>
+        <v>170</v>
       </c>
     </row>
     <row r="35" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>164</v>
+      </c>
       <c r="Q35" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
     </row>
     <row r="36" spans="2:17" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
-        <v>188</v>
+        <v>165</v>
       </c>
       <c r="P36" t="s">
-        <v>194</v>
+        <v>171</v>
       </c>
     </row>
     <row r="37" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
-        <v>184</v>
+        <v>161</v>
       </c>
       <c r="Q37" t="s">
-        <v>196</v>
+        <v>173</v>
       </c>
     </row>
     <row r="38" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
-        <v>198</v>
+        <v>175</v>
       </c>
     </row>
     <row r="39" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>179</v>
+        <v>156</v>
       </c>
     </row>
     <row r="40" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
-        <v>182</v>
+        <v>159</v>
       </c>
     </row>
     <row r="41" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>180</v>
+        <v>157</v>
       </c>
     </row>
     <row r="42" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
-        <v>191</v>
+        <v>168</v>
       </c>
     </row>
     <row r="43" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>181</v>
+        <v>158</v>
       </c>
     </row>
     <row r="44" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
-        <v>192</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -2510,16 +2453,16 @@
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
       <c r="B2" s="8"/>
     </row>
     <row r="3" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2528,10 +2471,10 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>120</v>
+        <v>103</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2539,7 +2482,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>122</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -2547,7 +2490,7 @@
         <v>13</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>122</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -2555,7 +2498,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>122</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -2563,7 +2506,7 @@
         <v>23</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2571,22 +2514,22 @@
         <v>21</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>124</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="B13" s="8"/>
     </row>
     <row r="14" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>134</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -2595,10 +2538,10 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>120</v>
+        <v>103</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -2606,7 +2549,7 @@
         <v>23</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -2614,7 +2557,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -2622,7 +2565,7 @@
         <v>16</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -2630,7 +2573,7 @@
         <v>24</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -2638,15 +2581,15 @@
         <v>33</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="20" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="B22" s="21" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -2668,7 +2611,7 @@
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I34" sqref="I34"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2699,7 +2642,7 @@
         <v>21</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="H1" t="s">
         <v>19</v>
@@ -2716,16 +2659,16 @@
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>201</v>
+        <v>177</v>
       </c>
       <c r="E2" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
       <c r="H2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="I2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -2739,10 +2682,10 @@
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>202</v>
+        <v>178</v>
       </c>
       <c r="E3" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2756,13 +2699,13 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>203</v>
+        <v>179</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>22</v>
       </c>
       <c r="H4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -2776,7 +2719,7 @@
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>204</v>
+        <v>180</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>20</v>
@@ -2795,10 +2738,10 @@
         <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>205</v>
+        <v>181</v>
       </c>
       <c r="E6" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -2812,10 +2755,10 @@
         <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>206</v>
+        <v>182</v>
       </c>
       <c r="E7" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -2829,10 +2772,10 @@
         <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>207</v>
+        <v>183</v>
       </c>
       <c r="E8" t="s">
-        <v>140</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -2846,10 +2789,10 @@
         <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>208</v>
+        <v>184</v>
       </c>
       <c r="E9" t="s">
-        <v>142</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -2863,13 +2806,13 @@
         <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>209</v>
+        <v>185</v>
       </c>
       <c r="E10" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
       <c r="G10" t="s">
-        <v>144</v>
+        <v>127</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -2883,10 +2826,10 @@
         <v>12</v>
       </c>
       <c r="D11" t="s">
-        <v>210</v>
+        <v>186</v>
       </c>
       <c r="E11" t="s">
-        <v>145</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -2900,10 +2843,10 @@
         <v>3</v>
       </c>
       <c r="D12" t="s">
-        <v>201</v>
+        <v>177</v>
       </c>
       <c r="E12" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -2917,10 +2860,10 @@
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>202</v>
+        <v>178</v>
       </c>
       <c r="E13" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -2934,10 +2877,10 @@
         <v>5</v>
       </c>
       <c r="D14" t="s">
-        <v>211</v>
+        <v>187</v>
       </c>
       <c r="E14" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -2951,10 +2894,10 @@
         <v>6</v>
       </c>
       <c r="D15" t="s">
-        <v>212</v>
+        <v>188</v>
       </c>
       <c r="E15" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -2968,10 +2911,10 @@
         <v>7</v>
       </c>
       <c r="D16" t="s">
-        <v>213</v>
+        <v>189</v>
       </c>
       <c r="E16" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -2985,10 +2928,10 @@
         <v>8</v>
       </c>
       <c r="D17" t="s">
-        <v>214</v>
+        <v>190</v>
       </c>
       <c r="E17" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -3002,10 +2945,10 @@
         <v>9</v>
       </c>
       <c r="D18" t="s">
-        <v>215</v>
+        <v>191</v>
       </c>
       <c r="E18" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="J18">
         <f>7644*12</f>
@@ -3023,10 +2966,10 @@
         <v>10</v>
       </c>
       <c r="D19" t="s">
-        <v>216</v>
+        <v>192</v>
       </c>
       <c r="E19" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="J19" s="6"/>
     </row>
@@ -3035,16 +2978,16 @@
         <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C20" t="s">
         <v>3</v>
       </c>
       <c r="D20" t="s">
-        <v>201</v>
+        <v>177</v>
       </c>
       <c r="E20" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -3052,16 +2995,16 @@
         <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>202</v>
+        <v>178</v>
       </c>
       <c r="E21" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3069,13 +3012,13 @@
         <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C22" t="s">
         <v>5</v>
       </c>
       <c r="D22" t="s">
-        <v>203</v>
+        <v>179</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>22</v>
@@ -3086,22 +3029,22 @@
         <v>2</v>
       </c>
       <c r="B23" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C23" t="s">
         <v>6</v>
       </c>
       <c r="D23" t="s">
-        <v>217</v>
+        <v>193</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>146</v>
+        <v>129</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="G23" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -3109,16 +3052,16 @@
         <v>2</v>
       </c>
       <c r="B24" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C24" t="s">
         <v>7</v>
       </c>
       <c r="D24" t="s">
-        <v>205</v>
+        <v>181</v>
       </c>
       <c r="E24" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3126,22 +3069,22 @@
         <v>2</v>
       </c>
       <c r="B25" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C25" t="s">
         <v>8</v>
       </c>
       <c r="D25" t="s">
-        <v>218</v>
+        <v>194</v>
       </c>
       <c r="E25" t="s">
-        <v>147</v>
+        <v>130</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="G25" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3149,22 +3092,22 @@
         <v>2</v>
       </c>
       <c r="B26" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C26" t="s">
         <v>9</v>
       </c>
       <c r="D26" t="s">
-        <v>219</v>
+        <v>195</v>
       </c>
       <c r="E26" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="G26" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -3172,16 +3115,16 @@
         <v>2</v>
       </c>
       <c r="B27" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C27" t="s">
         <v>10</v>
       </c>
       <c r="D27" t="s">
-        <v>208</v>
+        <v>184</v>
       </c>
       <c r="E27" t="s">
-        <v>142</v>
+        <v>125</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -3189,16 +3132,16 @@
         <v>2</v>
       </c>
       <c r="B28" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C28" t="s">
         <v>11</v>
       </c>
       <c r="D28" t="s">
-        <v>220</v>
+        <v>196</v>
       </c>
       <c r="E28" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -3206,118 +3149,118 @@
         <v>2</v>
       </c>
       <c r="B29" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C29" t="s">
         <v>12</v>
       </c>
       <c r="D29" t="s">
-        <v>210</v>
+        <v>186</v>
       </c>
       <c r="E29" t="s">
-        <v>145</v>
+        <v>128</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>156</v>
+        <v>139</v>
       </c>
       <c r="B30" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
       <c r="C30" t="s">
-        <v>158</v>
+        <v>141</v>
       </c>
       <c r="D30" t="s">
-        <v>221</v>
+        <v>197</v>
       </c>
       <c r="E30" t="s">
-        <v>170</v>
+        <v>147</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>156</v>
+        <v>139</v>
       </c>
       <c r="B31" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
       <c r="C31" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="D31" t="s">
-        <v>222</v>
+        <v>198</v>
       </c>
       <c r="E31" t="s">
-        <v>170</v>
+        <v>147</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>156</v>
+        <v>139</v>
       </c>
       <c r="B32" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
       <c r="C32" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="D32" t="s">
-        <v>223</v>
+        <v>199</v>
       </c>
       <c r="E32" t="s">
-        <v>170</v>
+        <v>147</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>156</v>
+        <v>139</v>
       </c>
       <c r="B33" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
       <c r="C33" t="s">
-        <v>164</v>
+        <v>144</v>
       </c>
       <c r="D33" t="s">
-        <v>224</v>
+        <v>200</v>
       </c>
       <c r="E33" t="s">
-        <v>170</v>
+        <v>147</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>156</v>
+        <v>139</v>
       </c>
       <c r="B34" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
       <c r="C34" t="s">
-        <v>166</v>
+        <v>145</v>
       </c>
       <c r="D34" t="s">
-        <v>225</v>
+        <v>201</v>
       </c>
       <c r="E34" t="s">
-        <v>170</v>
+        <v>147</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>156</v>
+        <v>139</v>
       </c>
       <c r="B35" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
       <c r="C35" t="s">
-        <v>168</v>
+        <v>146</v>
       </c>
       <c r="D35" t="s">
-        <v>226</v>
+        <v>202</v>
       </c>
       <c r="E35" t="s">
-        <v>170</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -3327,26 +3270,28 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62524B0A-320E-454A-8CBA-DBFB99CA201A}">
-  <sheetPr>
+  <sheetPr filterMode="1">
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:H71"/>
+  <dimension ref="A1:G71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I34" sqref="I34"/>
-      <selection pane="bottomLeft" activeCell="I71" sqref="I71"/>
+      <selection pane="bottomLeft" activeCell="D77" sqref="D77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" customWidth="1"/>
-    <col min="4" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -3363,15 +3308,15 @@
         <v>33</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="H1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>179</v>
       </c>
       <c r="B2" t="s">
         <v>25</v>
@@ -3386,15 +3331,15 @@
         <v>30</v>
       </c>
       <c r="F2" t="s">
-        <v>56</v>
-      </c>
-      <c r="H2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="G2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>179</v>
       </c>
       <c r="B3" t="s">
         <v>28</v>
@@ -3409,15 +3354,15 @@
         <v>31</v>
       </c>
       <c r="F3" t="s">
-        <v>56</v>
-      </c>
-      <c r="H3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="G3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>179</v>
       </c>
       <c r="B4" t="s">
         <v>32</v>
@@ -3432,92 +3377,92 @@
         <v>34</v>
       </c>
       <c r="F4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>180</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C5" t="s">
         <v>29</v>
       </c>
       <c r="D5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>180</v>
+      </c>
+      <c r="B6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" t="s">
         <v>52</v>
       </c>
-      <c r="E5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="D6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>180</v>
+      </c>
+      <c r="B7" t="s">
         <v>54</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>55</v>
       </c>
-      <c r="D6" t="s">
-        <v>56</v>
-      </c>
-      <c r="E6" t="s">
-        <v>56</v>
-      </c>
-      <c r="F6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>49</v>
-      </c>
-      <c r="B7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C7" t="s">
-        <v>58</v>
-      </c>
       <c r="D7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>180</v>
       </c>
       <c r="B8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C8" t="s">
         <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>180</v>
       </c>
       <c r="B9" t="s">
         <v>25</v>
@@ -3532,165 +3477,165 @@
         <v>30</v>
       </c>
       <c r="F9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>60</v>
+        <v>193</v>
       </c>
       <c r="B10" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C10" t="s">
         <v>29</v>
       </c>
       <c r="D10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>193</v>
+      </c>
+      <c r="B11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" t="s">
         <v>52</v>
       </c>
-      <c r="E10" t="s">
-        <v>53</v>
-      </c>
-      <c r="F10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>60</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="D11" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>193</v>
+      </c>
+      <c r="B12" t="s">
         <v>54</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>55</v>
       </c>
-      <c r="D11" t="s">
-        <v>56</v>
-      </c>
-      <c r="E11" t="s">
-        <v>56</v>
-      </c>
-      <c r="F11" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>60</v>
-      </c>
-      <c r="B12" t="s">
-        <v>57</v>
-      </c>
-      <c r="C12" t="s">
-        <v>58</v>
-      </c>
       <c r="D12" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E12" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>60</v>
+        <v>193</v>
       </c>
       <c r="B13" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C13" t="s">
         <v>29</v>
       </c>
       <c r="D13" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E13" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F13" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>74</v>
+        <v>181</v>
       </c>
       <c r="B14" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C14" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F14" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>74</v>
+        <v>181</v>
       </c>
       <c r="B15" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C15" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F15" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>74</v>
+        <v>181</v>
       </c>
       <c r="B16" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C16" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F16" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>74</v>
+        <v>181</v>
       </c>
       <c r="B17" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C17" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F17" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>74</v>
+        <v>181</v>
       </c>
       <c r="B18" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C18" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F18" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>74</v>
+        <v>181</v>
       </c>
       <c r="B19" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C19" t="s">
         <v>29</v>
@@ -3702,15 +3647,15 @@
         <v>34</v>
       </c>
       <c r="F19" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>77</v>
+        <v>182</v>
       </c>
       <c r="B20" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="C20" t="s">
         <v>29</v>
@@ -3722,55 +3667,55 @@
         <v>34</v>
       </c>
       <c r="F20" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>77</v>
+        <v>182</v>
       </c>
       <c r="B21" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C21" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D21" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E21" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F21" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>77</v>
+        <v>182</v>
       </c>
       <c r="B22" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C22" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D22" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E22" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F22" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>77</v>
+        <v>182</v>
       </c>
       <c r="B23" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C23" t="s">
         <v>29</v>
@@ -3782,35 +3727,35 @@
         <v>34</v>
       </c>
       <c r="F23" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>182</v>
+      </c>
+      <c r="B24" t="s">
         <v>77</v>
-      </c>
-      <c r="B24" t="s">
-        <v>84</v>
       </c>
       <c r="C24" t="s">
         <v>29</v>
       </c>
       <c r="D24" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E24" t="s">
         <v>30</v>
       </c>
       <c r="F24" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>78</v>
+        <v>194</v>
       </c>
       <c r="B25" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="C25" t="s">
         <v>29</v>
@@ -3822,35 +3767,35 @@
         <v>34</v>
       </c>
       <c r="F25" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>78</v>
+        <v>194</v>
       </c>
       <c r="B26" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C26" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D26" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E26" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F26" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>78</v>
+        <v>194</v>
       </c>
       <c r="B27" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C27" t="s">
         <v>29</v>
@@ -3862,235 +3807,235 @@
         <v>34</v>
       </c>
       <c r="F27" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>78</v>
+        <v>194</v>
       </c>
       <c r="B28" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C28" t="s">
         <v>29</v>
       </c>
       <c r="D28" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E28" t="s">
         <v>30</v>
       </c>
       <c r="F28" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>86</v>
+        <v>183</v>
       </c>
       <c r="B29" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="C29" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D29" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E29" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F29" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>86</v>
+        <v>183</v>
       </c>
       <c r="B30" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C30" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D30" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E30" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F30" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>86</v>
+        <v>183</v>
       </c>
       <c r="B31" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="C31" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D31" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E31" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F31" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>86</v>
+        <v>183</v>
       </c>
       <c r="B32" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="C32" t="s">
         <v>29</v>
       </c>
       <c r="D32" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E32" t="s">
         <v>30</v>
       </c>
       <c r="F32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>87</v>
+        <v>195</v>
       </c>
       <c r="B33" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="C33" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D33" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E33" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F33" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>87</v>
+        <v>195</v>
       </c>
       <c r="B34" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C34" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D34" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E34" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F34" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>87</v>
+        <v>195</v>
       </c>
       <c r="B35" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="C35" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D35" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E35" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F35" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>94</v>
+        <v>184</v>
       </c>
       <c r="B36" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="C36" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D36" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E36" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F36" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>94</v>
+        <v>184</v>
       </c>
       <c r="B37" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="C37" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D37" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E37" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F37" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>94</v>
+        <v>184</v>
       </c>
       <c r="B38" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C38" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D38" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E38" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F38" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>94</v>
+        <v>184</v>
       </c>
       <c r="B39" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="C39" t="s">
         <v>29</v>
@@ -4099,295 +4044,295 @@
         <v>31</v>
       </c>
       <c r="E39" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="F39" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>94</v>
+        <v>184</v>
       </c>
       <c r="B40" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="C40" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D40" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E40" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F40" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>48</v>
+        <v>185</v>
       </c>
       <c r="B41" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="C41" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D41" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E41" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F41" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>48</v>
+        <v>185</v>
       </c>
       <c r="B42" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C42" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D42" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E42" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F42" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>101</v>
+        <v>196</v>
       </c>
       <c r="B43" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="C43" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D43" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E43" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F43" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>101</v>
+        <v>196</v>
       </c>
       <c r="B44" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C44" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D44" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E44" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F44" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>101</v>
+        <v>196</v>
       </c>
       <c r="B45" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="C45" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D45" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E45" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F45" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>101</v>
+        <v>196</v>
       </c>
       <c r="B46" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="C46" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D46" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E46" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F46" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>101</v>
+        <v>196</v>
       </c>
       <c r="B47" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="C47" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D47" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E47" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F47" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>107</v>
+        <v>187</v>
       </c>
       <c r="B48" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="C48" t="s">
         <v>29</v>
       </c>
       <c r="D48" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E48" t="s">
         <v>30</v>
       </c>
       <c r="F48" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>107</v>
+        <v>187</v>
       </c>
       <c r="B49" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
       <c r="C49" t="s">
         <v>29</v>
       </c>
       <c r="D49" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E49" t="s">
         <v>30</v>
       </c>
       <c r="F49" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>106</v>
+        <v>188</v>
       </c>
       <c r="B50" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C50" t="s">
         <v>29</v>
       </c>
       <c r="D50" t="s">
+        <v>49</v>
+      </c>
+      <c r="E50" t="s">
+        <v>50</v>
+      </c>
+      <c r="F50" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>188</v>
+      </c>
+      <c r="B51" t="s">
+        <v>51</v>
+      </c>
+      <c r="C51" t="s">
         <v>52</v>
       </c>
-      <c r="E50" t="s">
-        <v>53</v>
-      </c>
-      <c r="F50" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>106</v>
-      </c>
-      <c r="B51" t="s">
+      <c r="D51" t="s">
+        <v>53</v>
+      </c>
+      <c r="E51" t="s">
+        <v>53</v>
+      </c>
+      <c r="F51" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>188</v>
+      </c>
+      <c r="B52" t="s">
         <v>54</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C52" t="s">
         <v>55</v>
       </c>
-      <c r="D51" t="s">
-        <v>56</v>
-      </c>
-      <c r="E51" t="s">
-        <v>56</v>
-      </c>
-      <c r="F51" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>106</v>
-      </c>
-      <c r="B52" t="s">
-        <v>57</v>
-      </c>
-      <c r="C52" t="s">
-        <v>58</v>
-      </c>
       <c r="D52" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E52" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F52" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>106</v>
+        <v>188</v>
       </c>
       <c r="B53" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C53" t="s">
         <v>29</v>
       </c>
       <c r="D53" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E53" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F53" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>106</v>
+        <v>188</v>
       </c>
       <c r="B54" t="s">
         <v>25</v>
@@ -4402,215 +4347,215 @@
         <v>30</v>
       </c>
       <c r="F54" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>108</v>
+        <v>189</v>
       </c>
       <c r="B55" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="C55" t="s">
         <v>29</v>
       </c>
       <c r="D55" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E55" t="s">
         <v>30</v>
       </c>
       <c r="F55" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>109</v>
+        <v>190</v>
       </c>
       <c r="B56" t="s">
-        <v>114</v>
+        <v>97</v>
       </c>
       <c r="C56" t="s">
         <v>29</v>
       </c>
       <c r="D56" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E56" t="s">
         <v>31</v>
       </c>
       <c r="F56" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>109</v>
+        <v>190</v>
       </c>
       <c r="B57" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
       <c r="C57" t="s">
         <v>29</v>
       </c>
       <c r="D57" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E57" t="s">
         <v>31</v>
       </c>
       <c r="F57" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>109</v>
+        <v>190</v>
       </c>
       <c r="B58" t="s">
-        <v>116</v>
+        <v>99</v>
       </c>
       <c r="C58" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D58" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E58" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F58" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>110</v>
+        <v>191</v>
       </c>
       <c r="B59" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="C59" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D59" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E59" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F59" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>110</v>
+        <v>191</v>
       </c>
       <c r="B60" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="C60" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D60" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E60" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F60" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>111</v>
+        <v>192</v>
       </c>
       <c r="B61" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="C61" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D61" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E61" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F61" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>111</v>
+        <v>192</v>
       </c>
       <c r="B62" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="C62" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D62" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E62" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F62" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>111</v>
+        <v>192</v>
       </c>
       <c r="B63" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C63" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D63" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E63" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F63" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>111</v>
+        <v>192</v>
       </c>
       <c r="B64" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="C64" t="s">
         <v>29</v>
       </c>
       <c r="D64" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E64" t="s">
         <v>31</v>
       </c>
       <c r="F64" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>159</v>
+        <v>197</v>
       </c>
       <c r="B65" t="s">
-        <v>171</v>
+        <v>148</v>
       </c>
       <c r="C65" t="s">
         <v>29</v>
@@ -4619,15 +4564,15 @@
         <v>30</v>
       </c>
       <c r="E65" t="s">
-        <v>172</v>
+        <v>149</v>
       </c>
       <c r="F65" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>161</v>
+        <v>198</v>
       </c>
       <c r="B66" t="s">
         <v>25</v>
@@ -4642,12 +4587,12 @@
         <v>30</v>
       </c>
       <c r="F66" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>163</v>
+        <v>199</v>
       </c>
       <c r="B67" t="s">
         <v>28</v>
@@ -4662,32 +4607,32 @@
         <v>31</v>
       </c>
       <c r="F67" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>165</v>
+        <v>200</v>
       </c>
       <c r="B68" t="s">
-        <v>173</v>
+        <v>150</v>
       </c>
       <c r="C68" t="s">
         <v>27</v>
       </c>
       <c r="D68" t="s">
-        <v>174</v>
+        <v>151</v>
       </c>
       <c r="E68" t="s">
         <v>30</v>
       </c>
       <c r="F68" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>167</v>
+        <v>201</v>
       </c>
       <c r="B69" t="s">
         <v>32</v>
@@ -4702,51 +4647,57 @@
         <v>34</v>
       </c>
       <c r="F69" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>167</v>
+        <v>201</v>
       </c>
       <c r="B70" t="s">
-        <v>175</v>
+        <v>152</v>
       </c>
       <c r="C70" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D70" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E70" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F70" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>169</v>
+        <v>202</v>
       </c>
       <c r="B71" t="s">
-        <v>176</v>
+        <v>153</v>
       </c>
       <c r="C71" t="s">
-        <v>177</v>
+        <v>154</v>
       </c>
       <c r="D71" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E71" t="s">
         <v>30</v>
       </c>
       <c r="F71" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F31" xr:uid="{62524B0A-320E-454A-8CBA-DBFB99CA201A}"/>
+  <autoFilter ref="A1:F71" xr:uid="{62524B0A-320E-454A-8CBA-DBFB99CA201A}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="JobDUTotals"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
@@ -4767,22 +4718,22 @@
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>145</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>140</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
@@ -4797,67 +4748,67 @@
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>142</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>147</v>
+        <v>130</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>146</v>
+        <v>129</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
started setting up gp scripts folder for rp arterial congestion subreport.
</commit_message>
<xml_diff>
--- a/gp-services/ReportOutPlanning.xlsx
+++ b/gp-services/ReportOutPlanning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dconly\GitRepos\PPA3\gp-services\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28460CA9-96AD-4DB9-9A2B-C60679167979}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01EB8F3A-5192-44F3-BFB5-6EF620EBA9C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FileStructure" sheetId="2" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="207">
   <si>
     <t>Program</t>
   </si>
@@ -677,6 +677,9 @@
   </si>
   <si>
     <t>functions and classes for updating JSON portions for charts used in multiple reports</t>
+  </si>
+  <si>
+    <t>ChartCount</t>
   </si>
 </sst>
 </file>
@@ -2124,7 +2127,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46217BC4-FCC5-4552-804D-D0F33949E3F0}">
   <dimension ref="A1:X44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+    <sheetView topLeftCell="A20" workbookViewId="0">
       <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
@@ -3273,12 +3276,12 @@
   <sheetPr filterMode="1">
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:G71"/>
+  <dimension ref="A1:H71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I34" sqref="I34"/>
-      <selection pane="bottomLeft" activeCell="D77" sqref="D77"/>
+      <selection pane="bottomLeft" activeCell="D75" sqref="D75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3289,9 +3292,10 @@
     <col min="4" max="4" width="25.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -3310,11 +3314,14 @@
       <c r="F1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>179</v>
       </c>
@@ -3333,11 +3340,15 @@
       <c r="F2" t="s">
         <v>53</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2">
+        <f>COUNTIF(B:B,B2)</f>
+        <v>4</v>
+      </c>
+      <c r="H2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>179</v>
       </c>
@@ -3356,11 +3367,15 @@
       <c r="F3" t="s">
         <v>53</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3">
+        <f t="shared" ref="G3:G66" si="0">COUNTIF(B:B,B3)</f>
+        <v>2</v>
+      </c>
+      <c r="H3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>179</v>
       </c>
@@ -3379,8 +3394,12 @@
       <c r="F4" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>180</v>
       </c>
@@ -3399,8 +3418,12 @@
       <c r="F5" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>180</v>
       </c>
@@ -3419,8 +3442,12 @@
       <c r="F6" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>180</v>
       </c>
@@ -3439,8 +3466,12 @@
       <c r="F7" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>180</v>
       </c>
@@ -3459,8 +3490,12 @@
       <c r="F8" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>180</v>
       </c>
@@ -3479,8 +3514,12 @@
       <c r="F9" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>193</v>
       </c>
@@ -3499,8 +3538,12 @@
       <c r="F10" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>193</v>
       </c>
@@ -3519,8 +3562,12 @@
       <c r="F11" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>193</v>
       </c>
@@ -3539,8 +3586,12 @@
       <c r="F12" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>193</v>
       </c>
@@ -3559,8 +3610,12 @@
       <c r="F13" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>181</v>
       </c>
@@ -3573,8 +3628,12 @@
       <c r="F14" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>181</v>
       </c>
@@ -3587,8 +3646,12 @@
       <c r="F15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>181</v>
       </c>
@@ -3601,8 +3664,12 @@
       <c r="F16" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>181</v>
       </c>
@@ -3615,8 +3682,12 @@
       <c r="F17" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>181</v>
       </c>
@@ -3629,8 +3700,12 @@
       <c r="F18" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>181</v>
       </c>
@@ -3649,8 +3724,12 @@
       <c r="F19" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G19">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>182</v>
       </c>
@@ -3669,8 +3748,12 @@
       <c r="F20" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G20">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>182</v>
       </c>
@@ -3689,8 +3772,12 @@
       <c r="F21" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G21">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>182</v>
       </c>
@@ -3709,8 +3796,12 @@
       <c r="F22" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G22">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>182</v>
       </c>
@@ -3729,8 +3820,12 @@
       <c r="F23" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G23">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>182</v>
       </c>
@@ -3749,8 +3844,12 @@
       <c r="F24" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G24">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>194</v>
       </c>
@@ -3769,8 +3868,12 @@
       <c r="F25" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G25">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>194</v>
       </c>
@@ -3789,8 +3892,12 @@
       <c r="F26" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G26">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>194</v>
       </c>
@@ -3809,8 +3916,12 @@
       <c r="F27" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G27">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>194</v>
       </c>
@@ -3829,8 +3940,12 @@
       <c r="F28" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G28">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>183</v>
       </c>
@@ -3849,8 +3964,12 @@
       <c r="F29" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G29">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>183</v>
       </c>
@@ -3869,8 +3988,12 @@
       <c r="F30" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G30">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>183</v>
       </c>
@@ -3889,8 +4012,12 @@
       <c r="F31" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G31">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>183</v>
       </c>
@@ -3909,8 +4036,12 @@
       <c r="F32" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G32">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>195</v>
       </c>
@@ -3929,8 +4060,12 @@
       <c r="F33" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G33">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>195</v>
       </c>
@@ -3949,8 +4084,12 @@
       <c r="F34" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G34">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>195</v>
       </c>
@@ -3969,8 +4108,12 @@
       <c r="F35" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G35">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>184</v>
       </c>
@@ -3989,8 +4132,12 @@
       <c r="F36" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G36">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>184</v>
       </c>
@@ -4009,8 +4156,12 @@
       <c r="F37" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G37">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>184</v>
       </c>
@@ -4029,8 +4180,12 @@
       <c r="F38" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G38">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>184</v>
       </c>
@@ -4049,8 +4204,12 @@
       <c r="F39" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G39">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>184</v>
       </c>
@@ -4069,8 +4228,12 @@
       <c r="F40" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G40">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>185</v>
       </c>
@@ -4089,8 +4252,12 @@
       <c r="F41" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G41">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>185</v>
       </c>
@@ -4109,8 +4276,12 @@
       <c r="F42" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G42">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>196</v>
       </c>
@@ -4129,8 +4300,12 @@
       <c r="F43" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G43">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>196</v>
       </c>
@@ -4149,8 +4324,12 @@
       <c r="F44" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G44">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>196</v>
       </c>
@@ -4169,8 +4348,12 @@
       <c r="F45" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G45">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>196</v>
       </c>
@@ -4189,8 +4372,12 @@
       <c r="F46" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G46">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>196</v>
       </c>
@@ -4209,8 +4396,12 @@
       <c r="F47" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G47">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>187</v>
       </c>
@@ -4229,8 +4420,12 @@
       <c r="F48" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G48">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>187</v>
       </c>
@@ -4249,8 +4444,12 @@
       <c r="F49" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G49">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>188</v>
       </c>
@@ -4269,8 +4468,12 @@
       <c r="F50" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G50">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>188</v>
       </c>
@@ -4289,8 +4492,12 @@
       <c r="F51" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G51">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>188</v>
       </c>
@@ -4309,8 +4516,12 @@
       <c r="F52" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G52">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>188</v>
       </c>
@@ -4329,8 +4540,12 @@
       <c r="F53" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G53">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>188</v>
       </c>
@@ -4349,8 +4564,12 @@
       <c r="F54" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G54">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>189</v>
       </c>
@@ -4369,8 +4588,12 @@
       <c r="F55" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G55">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>190</v>
       </c>
@@ -4389,8 +4612,12 @@
       <c r="F56" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G56">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>190</v>
       </c>
@@ -4409,8 +4636,12 @@
       <c r="F57" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G57">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>190</v>
       </c>
@@ -4429,8 +4660,12 @@
       <c r="F58" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G58">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>191</v>
       </c>
@@ -4449,8 +4684,12 @@
       <c r="F59" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G59">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>191</v>
       </c>
@@ -4469,8 +4708,12 @@
       <c r="F60" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G60">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>192</v>
       </c>
@@ -4489,8 +4732,12 @@
       <c r="F61" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G61">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>192</v>
       </c>
@@ -4509,8 +4756,12 @@
       <c r="F62" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G62">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>192</v>
       </c>
@@ -4529,8 +4780,12 @@
       <c r="F63" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G63">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>192</v>
       </c>
@@ -4549,8 +4804,12 @@
       <c r="F64" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G64">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>197</v>
       </c>
@@ -4569,8 +4828,12 @@
       <c r="F65" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G65">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>198</v>
       </c>
@@ -4589,8 +4852,12 @@
       <c r="F66" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G66">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>199</v>
       </c>
@@ -4609,8 +4876,12 @@
       <c r="F67" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G67">
+        <f t="shared" ref="G67:G71" si="1">COUNTIF(B:B,B67)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>200</v>
       </c>
@@ -4629,8 +4900,12 @@
       <c r="F68" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G68">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>201</v>
       </c>
@@ -4649,8 +4924,12 @@
       <c r="F69" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G69">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>201</v>
       </c>
@@ -4669,8 +4948,12 @@
       <c r="F70" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G70">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>202</v>
       </c>
@@ -4689,12 +4972,16 @@
       <c r="F71" t="s">
         <v>53</v>
       </c>
+      <c r="G71">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F71" xr:uid="{62524B0A-320E-454A-8CBA-DBFB99CA201A}">
-    <filterColumn colId="1">
+    <filterColumn colId="0">
       <filters>
-        <filter val="JobDUTotals"/>
+        <filter val="rp_artexp_cong"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
updated report out planning XLSX to list the JSON templates YY added for comm design program
</commit_message>
<xml_diff>
--- a/gp-services/ReportOutPlanning.xlsx
+++ b/gp-services/ReportOutPlanning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dconly\GitRepos\PPA3\gp-services\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01EB8F3A-5192-44F3-BFB5-6EF620EBA9C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2730AB47-7453-48AC-95C5-ECD482F277DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FileStructure" sheetId="2" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="212">
   <si>
     <t>Program</t>
   </si>
@@ -502,9 +502,6 @@
     <t>NaturePreservation</t>
   </si>
   <si>
-    <t>tbd as of 2/24/2022</t>
-  </si>
-  <si>
     <t>ModeSplit</t>
   </si>
   <si>
@@ -680,6 +677,24 @@
   </si>
   <si>
     <t>ChartCount</t>
+  </si>
+  <si>
+    <t>SACOG_{Community Design Program}_{CommDesign}_TransportationChoice_sample_dataSource.json</t>
+  </si>
+  <si>
+    <t>SACOG_{Community Design Program}_{CommDesign}_CompactDev_sample_dataSource.json</t>
+  </si>
+  <si>
+    <t>SACOG_{Community Design Program}_{CommDesign}_MixedUse_sample_dataSource.json</t>
+  </si>
+  <si>
+    <t>SACOG_{Community Design Program}_{CommDesign}_HousingChoice_sample_dataSource.json</t>
+  </si>
+  <si>
+    <t>SACOG_{Community Design Program}_{CommDesign}_ExistingAssets_sample_dataSource.json</t>
+  </si>
+  <si>
+    <t>SACOG_{Community Design Program}_{CommDesign}_NaturePreservation_sample_dataSource.json</t>
   </si>
 </sst>
 </file>
@@ -2305,128 +2320,128 @@
     <row r="25" spans="1:24" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="O28" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="P29" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="Q30" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="P31" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E32" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="Q32" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="33" spans="2:17" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="O33" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="34" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E34" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="P34" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="35" spans="2:17" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="Q35" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="36" spans="2:17" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="P36" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="37" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="Q37" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="38" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="39" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="40" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="41" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="42" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="43" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="44" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -2611,10 +2626,10 @@
   </sheetPr>
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I34" sqref="I34"/>
-      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomLeft" activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2662,7 +2677,7 @@
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E2" t="s">
         <v>119</v>
@@ -2685,7 +2700,7 @@
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E3" t="s">
         <v>119</v>
@@ -2702,7 +2717,7 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>22</v>
@@ -2722,7 +2737,7 @@
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>20</v>
@@ -2741,7 +2756,7 @@
         <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E6" t="s">
         <v>118</v>
@@ -2758,7 +2773,7 @@
         <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E7" t="s">
         <v>120</v>
@@ -2775,7 +2790,7 @@
         <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E8" t="s">
         <v>123</v>
@@ -2792,7 +2807,7 @@
         <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E9" t="s">
         <v>125</v>
@@ -2809,7 +2824,7 @@
         <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E10" t="s">
         <v>126</v>
@@ -2829,7 +2844,7 @@
         <v>12</v>
       </c>
       <c r="D11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E11" t="s">
         <v>128</v>
@@ -2846,7 +2861,7 @@
         <v>3</v>
       </c>
       <c r="D12" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E12" t="s">
         <v>119</v>
@@ -2863,7 +2878,7 @@
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E13" t="s">
         <v>119</v>
@@ -2880,7 +2895,7 @@
         <v>5</v>
       </c>
       <c r="D14" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E14" t="s">
         <v>133</v>
@@ -2897,7 +2912,7 @@
         <v>6</v>
       </c>
       <c r="D15" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E15" t="s">
         <v>134</v>
@@ -2914,7 +2929,7 @@
         <v>7</v>
       </c>
       <c r="D16" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E16" t="s">
         <v>135</v>
@@ -2931,7 +2946,7 @@
         <v>8</v>
       </c>
       <c r="D17" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E17" t="s">
         <v>136</v>
@@ -2948,7 +2963,7 @@
         <v>9</v>
       </c>
       <c r="D18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E18" t="s">
         <v>137</v>
@@ -2969,7 +2984,7 @@
         <v>10</v>
       </c>
       <c r="D19" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E19" t="s">
         <v>138</v>
@@ -2987,7 +3002,7 @@
         <v>3</v>
       </c>
       <c r="D20" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E20" t="s">
         <v>119</v>
@@ -3004,7 +3019,7 @@
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E21" t="s">
         <v>119</v>
@@ -3021,7 +3036,7 @@
         <v>5</v>
       </c>
       <c r="D22" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>22</v>
@@ -3038,7 +3053,7 @@
         <v>6</v>
       </c>
       <c r="D23" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>129</v>
@@ -3061,7 +3076,7 @@
         <v>7</v>
       </c>
       <c r="D24" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E24" t="s">
         <v>118</v>
@@ -3078,7 +3093,7 @@
         <v>8</v>
       </c>
       <c r="D25" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E25" t="s">
         <v>130</v>
@@ -3101,7 +3116,7 @@
         <v>9</v>
       </c>
       <c r="D26" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E26" t="s">
         <v>131</v>
@@ -3124,7 +3139,7 @@
         <v>10</v>
       </c>
       <c r="D27" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E27" t="s">
         <v>125</v>
@@ -3141,7 +3156,7 @@
         <v>11</v>
       </c>
       <c r="D28" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E28" t="s">
         <v>132</v>
@@ -3158,7 +3173,7 @@
         <v>12</v>
       </c>
       <c r="D29" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E29" t="s">
         <v>128</v>
@@ -3175,10 +3190,10 @@
         <v>141</v>
       </c>
       <c r="D30" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E30" t="s">
-        <v>147</v>
+        <v>206</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -3192,10 +3207,10 @@
         <v>142</v>
       </c>
       <c r="D31" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E31" t="s">
-        <v>147</v>
+        <v>207</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -3209,10 +3224,10 @@
         <v>143</v>
       </c>
       <c r="D32" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E32" t="s">
-        <v>147</v>
+        <v>208</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -3226,10 +3241,10 @@
         <v>144</v>
       </c>
       <c r="D33" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E33" t="s">
-        <v>147</v>
+        <v>209</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -3243,10 +3258,10 @@
         <v>145</v>
       </c>
       <c r="D34" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E34" t="s">
-        <v>147</v>
+        <v>210</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -3260,10 +3275,10 @@
         <v>146</v>
       </c>
       <c r="D35" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E35" t="s">
-        <v>147</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -3273,12 +3288,12 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62524B0A-320E-454A-8CBA-DBFB99CA201A}">
-  <sheetPr filterMode="1">
+  <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
   <dimension ref="A1:H71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I34" sqref="I34"/>
       <selection pane="bottomLeft" activeCell="D75" sqref="D75"/>
@@ -3315,15 +3330,15 @@
         <v>83</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B2" t="s">
         <v>25</v>
@@ -3348,9 +3363,9 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B3" t="s">
         <v>28</v>
@@ -3375,9 +3390,9 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B4" t="s">
         <v>32</v>
@@ -3401,7 +3416,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B5" t="s">
         <v>48</v>
@@ -3425,7 +3440,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B6" t="s">
         <v>51</v>
@@ -3449,7 +3464,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B7" t="s">
         <v>54</v>
@@ -3473,7 +3488,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B8" t="s">
         <v>61</v>
@@ -3497,7 +3512,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B9" t="s">
         <v>25</v>
@@ -3519,9 +3534,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B10" t="s">
         <v>48</v>
@@ -3543,9 +3558,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B11" t="s">
         <v>51</v>
@@ -3567,9 +3582,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B12" t="s">
         <v>54</v>
@@ -3591,9 +3606,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B13" t="s">
         <v>61</v>
@@ -3615,9 +3630,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B14" t="s">
         <v>63</v>
@@ -3633,9 +3648,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B15" t="s">
         <v>64</v>
@@ -3651,9 +3666,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B16" t="s">
         <v>67</v>
@@ -3669,9 +3684,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B17" t="s">
         <v>65</v>
@@ -3687,9 +3702,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B18" t="s">
         <v>66</v>
@@ -3705,9 +3720,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B19" t="s">
         <v>68</v>
@@ -3729,9 +3744,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B20" t="s">
         <v>73</v>
@@ -3753,9 +3768,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B21" t="s">
         <v>74</v>
@@ -3777,9 +3792,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B22" t="s">
         <v>75</v>
@@ -3801,9 +3816,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B23" t="s">
         <v>76</v>
@@ -3825,9 +3840,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B24" t="s">
         <v>77</v>
@@ -3849,9 +3864,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B25" t="s">
         <v>73</v>
@@ -3873,9 +3888,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B26" t="s">
         <v>75</v>
@@ -3897,9 +3912,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B27" t="s">
         <v>76</v>
@@ -3921,9 +3936,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B28" t="s">
         <v>77</v>
@@ -3945,9 +3960,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B29" t="s">
         <v>80</v>
@@ -3969,9 +3984,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B30" t="s">
         <v>81</v>
@@ -3993,9 +4008,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B31" t="s">
         <v>82</v>
@@ -4017,9 +4032,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B32" t="s">
         <v>84</v>
@@ -4041,9 +4056,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B33" t="s">
         <v>80</v>
@@ -4065,9 +4080,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B34" t="s">
         <v>81</v>
@@ -4089,9 +4104,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B35" t="s">
         <v>82</v>
@@ -4113,9 +4128,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B36" t="s">
         <v>85</v>
@@ -4137,9 +4152,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B37" t="s">
         <v>86</v>
@@ -4161,9 +4176,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B38" t="s">
         <v>87</v>
@@ -4185,9 +4200,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B39" t="s">
         <v>90</v>
@@ -4209,9 +4224,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B40" t="s">
         <v>88</v>
@@ -4233,9 +4248,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B41" t="s">
         <v>91</v>
@@ -4257,9 +4272,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B42" t="s">
         <v>54</v>
@@ -4281,9 +4296,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B43" t="s">
         <v>91</v>
@@ -4305,9 +4320,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B44" t="s">
         <v>54</v>
@@ -4329,9 +4344,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B45" t="s">
         <v>92</v>
@@ -4353,9 +4368,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B46" t="s">
         <v>93</v>
@@ -4377,9 +4392,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B47" t="s">
         <v>94</v>
@@ -4401,9 +4416,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B48" t="s">
         <v>95</v>
@@ -4425,9 +4440,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B49" t="s">
         <v>96</v>
@@ -4449,9 +4464,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B50" t="s">
         <v>48</v>
@@ -4473,9 +4488,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B51" t="s">
         <v>51</v>
@@ -4497,9 +4512,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B52" t="s">
         <v>54</v>
@@ -4521,9 +4536,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B53" t="s">
         <v>61</v>
@@ -4545,9 +4560,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B54" t="s">
         <v>25</v>
@@ -4569,9 +4584,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B55" t="s">
         <v>95</v>
@@ -4593,9 +4608,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B56" t="s">
         <v>97</v>
@@ -4617,9 +4632,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B57" t="s">
         <v>98</v>
@@ -4641,9 +4656,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B58" t="s">
         <v>99</v>
@@ -4665,9 +4680,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B59" t="s">
         <v>80</v>
@@ -4689,9 +4704,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B60" t="s">
         <v>100</v>
@@ -4713,9 +4728,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B61" t="s">
         <v>85</v>
@@ -4737,9 +4752,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B62" t="s">
         <v>86</v>
@@ -4761,9 +4776,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B63" t="s">
         <v>87</v>
@@ -4785,9 +4800,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B64" t="s">
         <v>101</v>
@@ -4809,12 +4824,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B65" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C65" t="s">
         <v>29</v>
@@ -4823,7 +4838,7 @@
         <v>30</v>
       </c>
       <c r="E65" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F65" t="s">
         <v>53</v>
@@ -4833,9 +4848,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B66" t="s">
         <v>25</v>
@@ -4857,9 +4872,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B67" t="s">
         <v>28</v>
@@ -4881,18 +4896,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B68" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C68" t="s">
         <v>27</v>
       </c>
       <c r="D68" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E68" t="s">
         <v>30</v>
@@ -4905,9 +4920,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B69" t="s">
         <v>32</v>
@@ -4929,12 +4944,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B70" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C70" t="s">
         <v>55</v>
@@ -4953,15 +4968,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B71" t="s">
+        <v>152</v>
+      </c>
+      <c r="C71" t="s">
         <v>153</v>
-      </c>
-      <c r="C71" t="s">
-        <v>154</v>
       </c>
       <c r="D71" t="s">
         <v>53</v>
@@ -4978,13 +4993,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F71" xr:uid="{62524B0A-320E-454A-8CBA-DBFB99CA201A}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="rp_artexp_cong"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:F71" xr:uid="{62524B0A-320E-454A-8CBA-DBFB99CA201A}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>